<commit_message>
Vaccine form fixed - link to children broken
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA6735C-4064-45D3-9010-3FD2AEFF4003}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693293B6-7A4B-4539-9CE2-067563248330}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -961,7 +961,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
@@ -1764,7 +1764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,9 +1918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Name change: MIFVIST -> MIF_VISIT
Same naming as other forms.
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693293B6-7A4B-4539-9CE2-067563248330}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53542BFF-DDEC-4163-BC7B-D00B6F622C31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,9 +411,6 @@
     <t>linked_visitdate</t>
   </si>
   <si>
-    <t>MIFVISIT</t>
-  </si>
-  <si>
     <t>ID = ?</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>LASTVISIT</t>
+  </si>
+  <si>
+    <t>MIF_VISIT</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1102,7 @@
         <v>125</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,25 +1732,25 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" t="s">
         <v>126</v>
       </c>
-      <c r="D19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>127</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
         <v>128</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
fixed linked table in cri visit
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA_LV/CRIANCA_LV.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE63E393-260C-4A51-9725-8A897D455BBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09417EB5-CF7B-4870-9740-D981E0CD6DCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -309,9 +309,6 @@
     <t>Children - launch visit</t>
   </si>
   <si>
-    <t>{REGIDC: data('REGIDC'), comsup: data('COMSUP'), parma: data('PARMA'), moma: data('MOMA')}</t>
-  </si>
-  <si>
     <t>linked_status</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t xml:space="preserve">text </t>
+  </si>
+  <si>
+    <t>{REGIDC: data('REGIDC'), comsup: data('COMSUP'), parma: data('PARMA'), moma: data('MOMA'), REGID: data('REGID')}</t>
   </si>
 </sst>
 </file>
@@ -1102,156 +1102,156 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
         <v>93</v>
-      </c>
-      <c r="F13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
         <v>97</v>
-      </c>
-      <c r="F15" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D17" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D19" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D22" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D23" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D24" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D25" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -1344,7 +1344,7 @@
         <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>77</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
@@ -1379,12 +1379,12 @@
         <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>76</v>
@@ -1408,12 +1408,12 @@
         <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -1437,12 +1437,12 @@
         <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
         <v>76</v>
@@ -1466,12 +1466,12 @@
         <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
         <v>76</v>
@@ -1495,12 +1495,12 @@
         <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>76</v>
@@ -1524,12 +1524,12 @@
         <v>77</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>76</v>
@@ -1553,12 +1553,12 @@
         <v>77</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -1582,12 +1582,12 @@
         <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
@@ -1611,12 +1611,12 @@
         <v>77</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
         <v>76</v>
@@ -1640,12 +1640,12 @@
         <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
         <v>76</v>
@@ -1669,12 +1669,12 @@
         <v>77</v>
       </c>
       <c r="I15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>76</v>
@@ -1698,12 +1698,12 @@
         <v>77</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
@@ -1727,28 +1727,28 @@
         <v>77</v>
       </c>
       <c r="I17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>76</v>
       </c>
       <c r="C19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" t="s">
         <v>127</v>
       </c>
-      <c r="D19" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>128</v>
       </c>
-      <c r="F19" t="s">
-        <v>129</v>
-      </c>
       <c r="G19" s="11" t="s">
         <v>77</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>77</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>79</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>25</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
@@ -1924,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2125,10 +2125,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -2191,10 +2191,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" t="s">
         <v>131</v>
-      </c>
-      <c r="B32" t="s">
-        <v>132</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>

</xml_diff>